<commit_message>
Randmoize the Email and remove it from the test data sheet
</commit_message>
<xml_diff>
--- a/Source/TestData/TestData.xlsx
+++ b/Source/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\habdelrahma2\eclipse-workspace2\AutomationTask\Source\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94321FC9-F249-44A9-A4CD-396B76EA0601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1811FA-B36C-4E5F-9187-9FF41A0F674B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="140" windowWidth="17320" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="39">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -142,27 +142,16 @@
   </si>
   <si>
     <t>An account using this email address has already been registered. Please enter a valid password or request a new one.</t>
-  </si>
-  <si>
-    <t>hagahassan1171@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,16 +174,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -473,84 +459,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
+      <c r="B2" t="s">
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
         <v>15</v>
       </c>
+      <c r="G2">
+        <v>67897</v>
+      </c>
       <c r="H2">
-        <v>67897</v>
-      </c>
-      <c r="I2">
         <v>1155654359</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -558,12 +538,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -571,7 +551,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -597,7 +577,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -626,7 +606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -652,7 +632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -681,7 +661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -707,7 +687,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -736,7 +716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -762,7 +742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -791,7 +771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>2</v>
       </c>
@@ -817,7 +797,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -921,9 +901,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{35EEC1F6-D5A6-40F3-8401-D2D3FD091D5C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>